<commit_message>
Consulta 2 Test completos
</commit_message>
<xml_diff>
--- a/Consulta2/AHP.xlsx
+++ b/Consulta2/AHP.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA7B2D1-CAC3-4B97-B657-F5DD3D727A49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4BB58CA-F55A-4161-92E9-ED9CF49A0AE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -223,28 +223,28 @@
     <t>1000kbTamaño aprox</t>
   </si>
   <si>
-    <t>0.002019</t>
-  </si>
-  <si>
-    <t>0.000667</t>
-  </si>
-  <si>
-    <t>0.002330</t>
-  </si>
-  <si>
     <t>0.002701</t>
   </si>
   <si>
     <t>0.001450</t>
   </si>
   <si>
-    <t>0.003881</t>
-  </si>
-  <si>
     <t>0.003665</t>
   </si>
   <si>
     <t>0.002951</t>
+  </si>
+  <si>
+    <t>0.001281</t>
+  </si>
+  <si>
+    <t>0.001057</t>
+  </si>
+  <si>
+    <t>0.002798</t>
+  </si>
+  <si>
+    <t>0.002329</t>
   </si>
 </sst>
 </file>
@@ -1659,6 +1659,9 @@
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="9" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -1741,6 +1744,33 @@
     <xf numFmtId="0" fontId="46" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="32" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="32" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="32" fillId="0" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="33" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1756,33 +1786,6 @@
     <xf numFmtId="10" fontId="33" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="32" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="32" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="32" fillId="0" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1807,9 +1810,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2232,17 +2232,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="36.6" x14ac:dyDescent="0.85">
-      <c r="A1" s="136" t="s">
+      <c r="A1" s="139" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="136"/>
-      <c r="C1" s="136"/>
-      <c r="D1" s="136"/>
-      <c r="E1" s="136"/>
-      <c r="F1" s="136"/>
-      <c r="G1" s="136"/>
-      <c r="H1" s="136"/>
-      <c r="I1" s="136"/>
+      <c r="B1" s="139"/>
+      <c r="C1" s="139"/>
+      <c r="D1" s="139"/>
+      <c r="E1" s="139"/>
+      <c r="F1" s="139"/>
+      <c r="G1" s="139"/>
+      <c r="H1" s="139"/>
+      <c r="I1" s="139"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -2267,10 +2267,10 @@
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="137" t="s">
+      <c r="A4" s="140" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="137"/>
+      <c r="B4" s="140"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="95" t="s">
@@ -2289,7 +2289,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="138" t="s">
+      <c r="D5" s="141" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="90" t="s">
@@ -2308,7 +2308,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="139"/>
+      <c r="D6" s="142"/>
       <c r="E6" s="91" t="s">
         <v>44</v>
       </c>
@@ -2325,7 +2325,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="139"/>
+      <c r="D7" s="142"/>
       <c r="E7" s="91" t="s">
         <v>45</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="139"/>
+      <c r="D8" s="142"/>
       <c r="E8" s="91" t="s">
         <v>46</v>
       </c>
@@ -2374,7 +2374,7 @@
         <v>4</v>
       </c>
       <c r="C10" s="1"/>
-      <c r="D10" s="140" t="s">
+      <c r="D10" s="143" t="s">
         <v>4</v>
       </c>
       <c r="E10" s="94"/>
@@ -2391,7 +2391,7 @@
         <v>3</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="D11" s="141"/>
+      <c r="D11" s="144"/>
       <c r="E11" s="135" t="s">
         <v>47</v>
       </c>
@@ -2408,7 +2408,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="1"/>
-      <c r="D12" s="141"/>
+      <c r="D12" s="144"/>
       <c r="E12" s="115" t="s">
         <v>48</v>
       </c>
@@ -2425,7 +2425,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="1"/>
-      <c r="D13" s="141"/>
+      <c r="D13" s="144"/>
       <c r="E13" s="115" t="s">
         <v>49</v>
       </c>
@@ -2438,7 +2438,7 @@
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="142"/>
+      <c r="D14" s="145"/>
       <c r="E14" s="92"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -2477,17 +2477,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="36.6" x14ac:dyDescent="0.85">
-      <c r="A1" s="143" t="s">
+      <c r="A1" s="146" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="143"/>
-      <c r="C1" s="143"/>
-      <c r="D1" s="143"/>
-      <c r="E1" s="143"/>
-      <c r="F1" s="143"/>
-      <c r="G1" s="143"/>
-      <c r="H1" s="143"/>
-      <c r="I1" s="143"/>
+      <c r="B1" s="146"/>
+      <c r="C1" s="146"/>
+      <c r="D1" s="146"/>
+      <c r="E1" s="146"/>
+      <c r="F1" s="146"/>
+      <c r="G1" s="146"/>
+      <c r="H1" s="146"/>
+      <c r="I1" s="146"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
@@ -2514,13 +2514,13 @@
     <row r="4" spans="1:9" ht="25.2" x14ac:dyDescent="0.6">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="144" t="s">
+      <c r="C4" s="147" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="144"/>
-      <c r="E4" s="144"/>
-      <c r="F4" s="144"/>
-      <c r="G4" s="144"/>
+      <c r="D4" s="147"/>
+      <c r="E4" s="147"/>
+      <c r="F4" s="147"/>
+      <c r="G4" s="147"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
     </row>
@@ -2538,13 +2538,13 @@
     <row r="6" spans="1:9" ht="16.2" x14ac:dyDescent="0.4">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
-      <c r="C6" s="145" t="s">
+      <c r="C6" s="148" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="146"/>
-      <c r="E6" s="146"/>
-      <c r="F6" s="146"/>
-      <c r="G6" s="147"/>
+      <c r="D6" s="149"/>
+      <c r="E6" s="149"/>
+      <c r="F6" s="149"/>
+      <c r="G6" s="150"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
@@ -2753,8 +2753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView topLeftCell="B29" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2772,22 +2772,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="30" x14ac:dyDescent="0.7">
-      <c r="A1" s="151" t="s">
+      <c r="A1" s="154" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="151"/>
-      <c r="C1" s="151"/>
-      <c r="D1" s="151"/>
-      <c r="E1" s="151"/>
-      <c r="F1" s="151"/>
-      <c r="G1" s="151"/>
-      <c r="H1" s="151"/>
-      <c r="I1" s="151"/>
-      <c r="J1" s="151"/>
-      <c r="K1" s="151"/>
-      <c r="L1" s="151"/>
-      <c r="M1" s="151"/>
-      <c r="N1" s="151"/>
+      <c r="B1" s="154"/>
+      <c r="C1" s="154"/>
+      <c r="D1" s="154"/>
+      <c r="E1" s="154"/>
+      <c r="F1" s="154"/>
+      <c r="G1" s="154"/>
+      <c r="H1" s="154"/>
+      <c r="I1" s="154"/>
+      <c r="J1" s="154"/>
+      <c r="K1" s="154"/>
+      <c r="L1" s="154"/>
+      <c r="M1" s="154"/>
+      <c r="N1" s="154"/>
     </row>
     <row r="2" spans="1:14" ht="30" x14ac:dyDescent="0.7">
       <c r="A2" s="128"/>
@@ -2830,20 +2830,20 @@
       <c r="B4" s="121">
         <v>4</v>
       </c>
-      <c r="C4" s="152" t="s">
+      <c r="C4" s="155" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="153"/>
-      <c r="E4" s="153"/>
-      <c r="F4" s="153"/>
-      <c r="G4" s="154"/>
+      <c r="D4" s="156"/>
+      <c r="E4" s="156"/>
+      <c r="F4" s="156"/>
+      <c r="G4" s="157"/>
       <c r="H4" s="12"/>
-      <c r="I4" s="152" t="s">
+      <c r="I4" s="155" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="153"/>
-      <c r="K4" s="153"/>
-      <c r="L4" s="154"/>
+      <c r="J4" s="156"/>
+      <c r="K4" s="156"/>
+      <c r="L4" s="157"/>
       <c r="M4" s="12"/>
       <c r="N4" s="53" t="s">
         <v>16</v>
@@ -2866,7 +2866,7 @@
       <c r="N5" s="2"/>
     </row>
     <row r="6" spans="1:14" ht="15.6" x14ac:dyDescent="0.4">
-      <c r="A6" s="155" t="s">
+      <c r="A6" s="158" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="14"/>
@@ -2908,7 +2908,7 @@
       <c r="N6" s="15"/>
     </row>
     <row r="7" spans="1:14" ht="18.600000000000001" x14ac:dyDescent="0.45">
-      <c r="A7" s="156"/>
+      <c r="A7" s="159"/>
       <c r="B7" s="17"/>
       <c r="C7" s="51" t="str">
         <f>D6</f>
@@ -2950,7 +2950,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="18.600000000000001" x14ac:dyDescent="0.45">
-      <c r="A8" s="156"/>
+      <c r="A8" s="159"/>
       <c r="B8" s="17"/>
       <c r="C8" s="51" t="str">
         <f>E6</f>
@@ -2992,7 +2992,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="18.600000000000001" x14ac:dyDescent="0.45">
-      <c r="A9" s="156"/>
+      <c r="A9" s="159"/>
       <c r="B9" s="17"/>
       <c r="C9" s="51" t="str">
         <f>F6</f>
@@ -3034,7 +3034,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="18.600000000000001" x14ac:dyDescent="0.45">
-      <c r="A10" s="156"/>
+      <c r="A10" s="159"/>
       <c r="B10" s="17"/>
       <c r="C10" s="51" t="str">
         <f>G6</f>
@@ -3076,7 +3076,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="18.600000000000001" x14ac:dyDescent="0.45">
-      <c r="A11" s="156"/>
+      <c r="A11" s="159"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="72"/>
@@ -3092,7 +3092,7 @@
       <c r="N11" s="74"/>
     </row>
     <row r="12" spans="1:14" ht="18.600000000000001" x14ac:dyDescent="0.45">
-      <c r="A12" s="157"/>
+      <c r="A12" s="160"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="59">
@@ -3192,7 +3192,7 @@
       <c r="N15" s="2"/>
     </row>
     <row r="16" spans="1:14" ht="16.2" x14ac:dyDescent="0.4">
-      <c r="A16" s="148" t="s">
+      <c r="A16" s="151" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="15"/>
@@ -3230,7 +3230,7 @@
       <c r="N16" s="15"/>
     </row>
     <row r="17" spans="1:14" ht="18.600000000000001" x14ac:dyDescent="0.45">
-      <c r="A17" s="149"/>
+      <c r="A17" s="152"/>
       <c r="B17" s="2"/>
       <c r="C17" s="96" t="str">
         <f>D16</f>
@@ -3269,7 +3269,7 @@
       </c>
     </row>
     <row r="18" spans="1:14" ht="18.600000000000001" x14ac:dyDescent="0.45">
-      <c r="A18" s="149"/>
+      <c r="A18" s="152"/>
       <c r="B18" s="2"/>
       <c r="C18" s="96" t="str">
         <f>E16</f>
@@ -3308,7 +3308,7 @@
       </c>
     </row>
     <row r="19" spans="1:14" ht="18.600000000000001" x14ac:dyDescent="0.45">
-      <c r="A19" s="149"/>
+      <c r="A19" s="152"/>
       <c r="B19" s="2"/>
       <c r="C19" s="96" t="str">
         <f>F16</f>
@@ -3347,7 +3347,7 @@
       </c>
     </row>
     <row r="20" spans="1:14" ht="18.600000000000001" x14ac:dyDescent="0.45">
-      <c r="A20" s="149"/>
+      <c r="A20" s="152"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="58"/>
@@ -3363,7 +3363,7 @@
       <c r="N20" s="61"/>
     </row>
     <row r="21" spans="1:14" ht="18.600000000000001" x14ac:dyDescent="0.45">
-      <c r="A21" s="150"/>
+      <c r="A21" s="153"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="59">
@@ -3453,7 +3453,7 @@
       <c r="N24" s="2"/>
     </row>
     <row r="25" spans="1:14" ht="16.2" x14ac:dyDescent="0.4">
-      <c r="A25" s="148" t="s">
+      <c r="A25" s="151" t="s">
         <v>19</v>
       </c>
       <c r="B25" s="15"/>
@@ -3491,7 +3491,7 @@
       <c r="N25" s="15"/>
     </row>
     <row r="26" spans="1:14" ht="18.600000000000001" x14ac:dyDescent="0.45">
-      <c r="A26" s="149"/>
+      <c r="A26" s="152"/>
       <c r="B26" s="2"/>
       <c r="C26" s="111" t="str">
         <f>C17</f>
@@ -3506,7 +3506,7 @@
       <c r="F26" s="57">
         <v>1</v>
       </c>
-      <c r="G26" s="183">
+      <c r="G26" s="136">
         <v>1</v>
       </c>
       <c r="H26" s="58"/>
@@ -3530,7 +3530,7 @@
       </c>
     </row>
     <row r="27" spans="1:14" ht="18.600000000000001" x14ac:dyDescent="0.45">
-      <c r="A27" s="149"/>
+      <c r="A27" s="152"/>
       <c r="B27" s="2"/>
       <c r="C27" s="111" t="str">
         <f>C18</f>
@@ -3545,7 +3545,7 @@
       <c r="F27" s="57">
         <v>1</v>
       </c>
-      <c r="G27" s="183">
+      <c r="G27" s="136">
         <v>1</v>
       </c>
       <c r="H27" s="58"/>
@@ -3569,7 +3569,7 @@
       </c>
     </row>
     <row r="28" spans="1:14" ht="18.600000000000001" x14ac:dyDescent="0.45">
-      <c r="A28" s="149"/>
+      <c r="A28" s="152"/>
       <c r="B28" s="2"/>
       <c r="C28" s="111" t="str">
         <f>C19</f>
@@ -3584,7 +3584,7 @@
       <c r="F28" s="56">
         <v>1</v>
       </c>
-      <c r="G28" s="183">
+      <c r="G28" s="136">
         <v>1</v>
       </c>
       <c r="H28" s="58"/>
@@ -3608,7 +3608,7 @@
       </c>
     </row>
     <row r="29" spans="1:14" ht="18.600000000000001" x14ac:dyDescent="0.45">
-      <c r="A29" s="149"/>
+      <c r="A29" s="152"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="58"/>
@@ -3624,7 +3624,7 @@
       <c r="N29" s="61"/>
     </row>
     <row r="30" spans="1:14" ht="18.600000000000001" x14ac:dyDescent="0.45">
-      <c r="A30" s="150"/>
+      <c r="A30" s="153"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="59">
@@ -3716,7 +3716,7 @@
       <c r="N33" s="2"/>
     </row>
     <row r="34" spans="1:14" ht="16.2" x14ac:dyDescent="0.4">
-      <c r="A34" s="148" t="s">
+      <c r="A34" s="151" t="s">
         <v>19</v>
       </c>
       <c r="B34" s="15"/>
@@ -3756,7 +3756,7 @@
       <c r="N34" s="15"/>
     </row>
     <row r="35" spans="1:14" ht="18.600000000000001" x14ac:dyDescent="0.45">
-      <c r="A35" s="149"/>
+      <c r="A35" s="152"/>
       <c r="B35" s="2"/>
       <c r="C35" s="111" t="str">
         <f>C17</f>
@@ -3769,7 +3769,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="F35" s="57">
-        <v>0.14285714285714285</v>
+        <v>0.2</v>
       </c>
       <c r="G35" s="58" t="s">
         <v>56</v>
@@ -3779,7 +3779,7 @@
       </c>
       <c r="I35" s="59">
         <f t="shared" ref="I35:K37" si="4">IF(ISERROR(D35/D$39),0,D35/D$39)</f>
-        <v>9.0909090909090912E-2</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="J35" s="59">
         <f t="shared" si="4"/>
@@ -3787,17 +3787,17 @@
       </c>
       <c r="K35" s="59">
         <f t="shared" si="4"/>
-        <v>0.10909090909090909</v>
+        <v>0.14634146341463414</v>
       </c>
       <c r="L35" s="58"/>
       <c r="M35" s="58"/>
       <c r="N35" s="60">
         <f>AVERAGE(I35:K35)</f>
-        <v>8.1818181818181804E-2</v>
+        <v>0.10096903999343025</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="18.600000000000001" x14ac:dyDescent="0.45">
-      <c r="A36" s="149"/>
+      <c r="A36" s="152"/>
       <c r="B36" s="2"/>
       <c r="C36" s="111" t="str">
         <f>C18</f>
@@ -3812,15 +3812,15 @@
       <c r="F36" s="57">
         <v>0.16666666666666666</v>
       </c>
-      <c r="G36" s="185" t="s">
+      <c r="G36" s="138" t="s">
+        <v>63</v>
+      </c>
+      <c r="H36" s="58" t="s">
         <v>66</v>
-      </c>
-      <c r="H36" s="58" t="s">
-        <v>70</v>
       </c>
       <c r="I36" s="59">
         <f t="shared" si="4"/>
-        <v>0.27272727272727271</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="J36" s="59">
         <f t="shared" si="4"/>
@@ -3828,24 +3828,24 @@
       </c>
       <c r="K36" s="59">
         <f t="shared" si="4"/>
-        <v>0.12727272727272726</v>
+        <v>0.12195121951219512</v>
       </c>
       <c r="L36" s="58"/>
       <c r="M36" s="58"/>
       <c r="N36" s="60">
         <f>AVERAGE(I36:K36)</f>
-        <v>0.1787878787878788</v>
+        <v>0.19721606306972161</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="18.600000000000001" x14ac:dyDescent="0.45">
-      <c r="A37" s="149"/>
+      <c r="A37" s="152"/>
       <c r="B37" s="2"/>
       <c r="C37" s="111" t="str">
         <f>C19</f>
         <v>Aes-256-cbc</v>
       </c>
       <c r="D37" s="57">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E37" s="57">
         <v>6</v>
@@ -3853,15 +3853,15 @@
       <c r="F37" s="57">
         <v>1</v>
       </c>
-      <c r="G37" s="185" t="s">
-        <v>63</v>
+      <c r="G37" s="138" t="s">
+        <v>67</v>
       </c>
       <c r="H37" s="58" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="I37" s="59">
         <f t="shared" si="4"/>
-        <v>0.63636363636363635</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="J37" s="59">
         <f t="shared" si="4"/>
@@ -3869,17 +3869,17 @@
       </c>
       <c r="K37" s="59">
         <f t="shared" si="4"/>
-        <v>0.76363636363636367</v>
+        <v>0.73170731707317072</v>
       </c>
       <c r="L37" s="58"/>
       <c r="M37" s="58"/>
       <c r="N37" s="60">
         <f>AVERAGE(I37:K37)</f>
-        <v>0.73939393939393938</v>
+        <v>0.70181489693684806</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="18.600000000000001" x14ac:dyDescent="0.45">
-      <c r="A38" s="149"/>
+      <c r="A38" s="152"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="58"/>
@@ -3895,12 +3895,12 @@
       <c r="N38" s="61"/>
     </row>
     <row r="39" spans="1:14" ht="18.600000000000001" x14ac:dyDescent="0.45">
-      <c r="A39" s="150"/>
+      <c r="A39" s="153"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="59">
         <f>SUM(D35:D37)</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E39" s="59">
         <f>SUM(E35:E37)</f>
@@ -3908,9 +3908,9 @@
       </c>
       <c r="F39" s="59">
         <f>SUM(F35:F37)</f>
-        <v>1.3095238095238095</v>
-      </c>
-      <c r="G39" s="184"/>
+        <v>1.3666666666666667</v>
+      </c>
+      <c r="G39" s="137"/>
       <c r="H39" s="58"/>
       <c r="I39" s="59">
         <f>SUM(I35:I37)</f>
@@ -3987,7 +3987,7 @@
       <c r="N42" s="2"/>
     </row>
     <row r="43" spans="1:14" ht="16.2" x14ac:dyDescent="0.4">
-      <c r="A43" s="148" t="s">
+      <c r="A43" s="151" t="s">
         <v>19</v>
       </c>
       <c r="B43" s="15"/>
@@ -4027,7 +4027,7 @@
       <c r="N43" s="15"/>
     </row>
     <row r="44" spans="1:14" ht="18.600000000000001" x14ac:dyDescent="0.45">
-      <c r="A44" s="149"/>
+      <c r="A44" s="152"/>
       <c r="B44" s="2"/>
       <c r="C44" s="111" t="str">
         <f>C17</f>
@@ -4068,7 +4068,7 @@
       </c>
     </row>
     <row r="45" spans="1:14" ht="18.600000000000001" x14ac:dyDescent="0.45">
-      <c r="A45" s="149"/>
+      <c r="A45" s="152"/>
       <c r="B45" s="2"/>
       <c r="C45" s="111" t="str">
         <f>C18</f>
@@ -4084,10 +4084,10 @@
         <v>0.14285714285714285</v>
       </c>
       <c r="G45" s="58" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H45" s="58" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="I45" s="59">
         <f t="shared" si="5"/>
@@ -4109,7 +4109,7 @@
       </c>
     </row>
     <row r="46" spans="1:14" ht="18.600000000000001" x14ac:dyDescent="0.45">
-      <c r="A46" s="149"/>
+      <c r="A46" s="152"/>
       <c r="B46" s="2"/>
       <c r="C46" s="111" t="str">
         <f>C19</f>
@@ -4125,10 +4125,10 @@
         <v>1</v>
       </c>
       <c r="G46" s="58" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="H46" s="58" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="I46" s="59">
         <f t="shared" si="5"/>
@@ -4150,7 +4150,7 @@
       </c>
     </row>
     <row r="47" spans="1:14" ht="18.600000000000001" x14ac:dyDescent="0.45">
-      <c r="A47" s="149"/>
+      <c r="A47" s="152"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="58"/>
@@ -4166,7 +4166,7 @@
       <c r="N47" s="61"/>
     </row>
     <row r="48" spans="1:14" ht="18.600000000000001" x14ac:dyDescent="0.45">
-      <c r="A48" s="150"/>
+      <c r="A48" s="153"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="59">
@@ -4249,23 +4249,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="36.6" x14ac:dyDescent="0.85">
-      <c r="A1" s="143" t="s">
+      <c r="A1" s="146" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="143"/>
-      <c r="C1" s="143"/>
-      <c r="D1" s="143"/>
-      <c r="E1" s="143"/>
-      <c r="F1" s="143"/>
-      <c r="G1" s="143"/>
-      <c r="H1" s="143"/>
-      <c r="I1" s="143"/>
-      <c r="J1" s="143"/>
-      <c r="K1" s="143"/>
-      <c r="L1" s="143"/>
-      <c r="M1" s="143"/>
-      <c r="N1" s="143"/>
-      <c r="O1" s="143"/>
+      <c r="B1" s="146"/>
+      <c r="C1" s="146"/>
+      <c r="D1" s="146"/>
+      <c r="E1" s="146"/>
+      <c r="F1" s="146"/>
+      <c r="G1" s="146"/>
+      <c r="H1" s="146"/>
+      <c r="I1" s="146"/>
+      <c r="J1" s="146"/>
+      <c r="K1" s="146"/>
+      <c r="L1" s="146"/>
+      <c r="M1" s="146"/>
+      <c r="N1" s="146"/>
+      <c r="O1" s="146"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
@@ -4406,7 +4406,7 @@
       <c r="AA5" s="2"/>
     </row>
     <row r="6" spans="1:27" ht="17.399999999999999" x14ac:dyDescent="0.45">
-      <c r="A6" s="171" t="s">
+      <c r="A6" s="169" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="52" t="str">
@@ -4423,17 +4423,17 @@
         <v>4.2937853107344637</v>
       </c>
       <c r="F6" s="63"/>
-      <c r="G6" s="166">
+      <c r="G6" s="164">
         <f>SUM(E6:E9)/Matrices!$B$4</f>
         <v>4.1506906182569878</v>
       </c>
       <c r="H6" s="63"/>
-      <c r="I6" s="166">
+      <c r="I6" s="164">
         <f>IF($C$11=Matrices!$B$4,0,(G6-Matrices!$B$4)/(Matrices!$B$4-1))</f>
         <v>5.0230206085662608E-2</v>
       </c>
       <c r="J6" s="63"/>
-      <c r="K6" s="169">
+      <c r="K6" s="167">
         <f>IF(I6=0,0,I6/HLOOKUP(Matrices!$B$4,$R$6:$AA$7,2,0))</f>
         <v>5.6438433804115291E-2</v>
       </c>
@@ -4477,7 +4477,7 @@
       </c>
     </row>
     <row r="7" spans="1:27" ht="17.399999999999999" x14ac:dyDescent="0.45">
-      <c r="A7" s="172"/>
+      <c r="A7" s="170"/>
       <c r="B7" s="52" t="str">
         <f>Datos!E6</f>
         <v>Integridad en el almacenamiento</v>
@@ -4492,11 +4492,11 @@
         <v>4.1875</v>
       </c>
       <c r="F7" s="63"/>
-      <c r="G7" s="167"/>
+      <c r="G7" s="165"/>
       <c r="H7" s="63"/>
-      <c r="I7" s="167"/>
+      <c r="I7" s="165"/>
       <c r="J7" s="63"/>
-      <c r="K7" s="170"/>
+      <c r="K7" s="168"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -4537,7 +4537,7 @@
       </c>
     </row>
     <row r="8" spans="1:27" ht="17.399999999999999" x14ac:dyDescent="0.45">
-      <c r="A8" s="172"/>
+      <c r="A8" s="170"/>
       <c r="B8" s="52" t="str">
         <f>Datos!E7</f>
         <v>Bajo tiempo procesamiento cifrado</v>
@@ -4552,11 +4552,11 @@
         <v>4.0903790087463552</v>
       </c>
       <c r="F8" s="63"/>
-      <c r="G8" s="167"/>
+      <c r="G8" s="165"/>
       <c r="H8" s="63"/>
-      <c r="I8" s="167"/>
+      <c r="I8" s="165"/>
       <c r="J8" s="63"/>
-      <c r="K8" s="170"/>
+      <c r="K8" s="168"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
@@ -4575,7 +4575,7 @@
       <c r="AA8" s="2"/>
     </row>
     <row r="9" spans="1:27" ht="17.399999999999999" x14ac:dyDescent="0.45">
-      <c r="A9" s="172"/>
+      <c r="A9" s="170"/>
       <c r="B9" s="52" t="str">
         <f>Datos!E8</f>
         <v>Bajo tiempo procesamiento descifrado</v>
@@ -4590,11 +4590,11 @@
         <v>4.0310981535471324</v>
       </c>
       <c r="F9" s="63"/>
-      <c r="G9" s="168"/>
+      <c r="G9" s="166"/>
       <c r="H9" s="63"/>
-      <c r="I9" s="168"/>
+      <c r="I9" s="166"/>
       <c r="J9" s="63"/>
-      <c r="K9" s="174"/>
+      <c r="K9" s="172"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
@@ -4613,7 +4613,7 @@
       <c r="AA9" s="2"/>
     </row>
     <row r="10" spans="1:27" ht="17.399999999999999" x14ac:dyDescent="0.45">
-      <c r="A10" s="172"/>
+      <c r="A10" s="170"/>
       <c r="B10" s="2"/>
       <c r="C10" s="78"/>
       <c r="D10" s="78"/>
@@ -4642,7 +4642,7 @@
       <c r="AA10" s="2"/>
     </row>
     <row r="11" spans="1:27" ht="17.399999999999999" x14ac:dyDescent="0.45">
-      <c r="A11" s="173"/>
+      <c r="A11" s="171"/>
       <c r="B11" s="2"/>
       <c r="C11" s="64">
         <f>SUM(C6:C9)</f>
@@ -4766,7 +4766,7 @@
       <c r="AA14" s="2"/>
     </row>
     <row r="15" spans="1:27" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="158" t="s">
+      <c r="A15" s="161" t="s">
         <v>27</v>
       </c>
       <c r="B15" s="98" t="str">
@@ -4783,17 +4783,17 @@
         <v>3.0139435511076127</v>
       </c>
       <c r="F15" s="63"/>
-      <c r="G15" s="166">
+      <c r="G15" s="164">
         <f>SUM(E15:E17)/Matrices!$B$15</f>
         <v>3.0070303834347594</v>
       </c>
       <c r="H15" s="63"/>
-      <c r="I15" s="166">
+      <c r="I15" s="164">
         <f>IF($C$19=Matrices!$B$15,0,(G15-Matrices!$B$15)/(Matrices!$B$15-1))</f>
         <v>3.5151917173796843E-3</v>
       </c>
       <c r="J15" s="63"/>
-      <c r="K15" s="169">
+      <c r="K15" s="167">
         <f>IF(I15=0,0,I15/HLOOKUP(Matrices!$B$15,$R$6:$AA$7,2,0))</f>
         <v>6.0606753747925596E-3</v>
       </c>
@@ -4804,7 +4804,7 @@
       <c r="P15" s="2"/>
     </row>
     <row r="16" spans="1:27" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="159"/>
+      <c r="A16" s="162"/>
       <c r="B16" s="98" t="str">
         <f>Datos!E12</f>
         <v>Camellia-256-cbc</v>
@@ -4819,11 +4819,11 @@
         <v>3.0017862217350708</v>
       </c>
       <c r="F16" s="63"/>
-      <c r="G16" s="167"/>
+      <c r="G16" s="165"/>
       <c r="H16" s="63"/>
-      <c r="I16" s="167"/>
+      <c r="I16" s="165"/>
       <c r="J16" s="63"/>
-      <c r="K16" s="170"/>
+      <c r="K16" s="168"/>
       <c r="L16" s="63"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
@@ -4831,7 +4831,7 @@
       <c r="P16" s="2"/>
     </row>
     <row r="17" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="159"/>
+      <c r="A17" s="162"/>
       <c r="B17" s="98" t="str">
         <f>Datos!E13</f>
         <v>Aes-256-cbc</v>
@@ -4846,11 +4846,11 @@
         <v>3.0053613774615942</v>
       </c>
       <c r="F17" s="63"/>
-      <c r="G17" s="168"/>
+      <c r="G17" s="166"/>
       <c r="H17" s="63"/>
-      <c r="I17" s="168"/>
+      <c r="I17" s="166"/>
       <c r="J17" s="63"/>
-      <c r="K17" s="170"/>
+      <c r="K17" s="168"/>
       <c r="L17" s="63"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -4858,7 +4858,7 @@
       <c r="P17" s="2"/>
     </row>
     <row r="18" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="159"/>
+      <c r="A18" s="162"/>
       <c r="B18" s="97"/>
       <c r="C18" s="78"/>
       <c r="D18" s="78"/>
@@ -4876,7 +4876,7 @@
       <c r="P18" s="2"/>
     </row>
     <row r="19" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="160"/>
+      <c r="A19" s="163"/>
       <c r="B19" s="97"/>
       <c r="C19" s="64">
         <f>SUM(C15:C17)</f>
@@ -4956,7 +4956,7 @@
       <c r="P22" s="2"/>
     </row>
     <row r="23" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="158" t="s">
+      <c r="A23" s="161" t="s">
         <v>27</v>
       </c>
       <c r="B23" s="98" t="str">
@@ -4973,17 +4973,17 @@
         <v>3</v>
       </c>
       <c r="F23" s="66"/>
-      <c r="G23" s="161">
+      <c r="G23" s="173">
         <f>SUM(E23:E25)/Matrices!$B$15</f>
         <v>3</v>
       </c>
       <c r="H23" s="66"/>
-      <c r="I23" s="161">
+      <c r="I23" s="173">
         <f>IF($C$27=Matrices!$B$15,0,(G23-Matrices!$B$15)/(Matrices!$B$15-1))</f>
         <v>0</v>
       </c>
       <c r="J23" s="66"/>
-      <c r="K23" s="164">
+      <c r="K23" s="176">
         <f>IF(I23=0,0,I23/HLOOKUP(Matrices!$B$15,$R$6:$AA$7,2,0))</f>
         <v>0</v>
       </c>
@@ -4994,7 +4994,7 @@
       <c r="P23" s="2"/>
     </row>
     <row r="24" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="159"/>
+      <c r="A24" s="162"/>
       <c r="B24" s="98" t="str">
         <f>B16</f>
         <v>Camellia-256-cbc</v>
@@ -5009,11 +5009,11 @@
         <v>3</v>
       </c>
       <c r="F24" s="66"/>
-      <c r="G24" s="162"/>
+      <c r="G24" s="174"/>
       <c r="H24" s="66"/>
-      <c r="I24" s="162"/>
+      <c r="I24" s="174"/>
       <c r="J24" s="66"/>
-      <c r="K24" s="165"/>
+      <c r="K24" s="177"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
@@ -5021,7 +5021,7 @@
       <c r="P24" s="2"/>
     </row>
     <row r="25" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="159"/>
+      <c r="A25" s="162"/>
       <c r="B25" s="98" t="str">
         <f>B17</f>
         <v>Aes-256-cbc</v>
@@ -5036,11 +5036,11 @@
         <v>3</v>
       </c>
       <c r="F25" s="66"/>
-      <c r="G25" s="163"/>
+      <c r="G25" s="175"/>
       <c r="H25" s="66"/>
-      <c r="I25" s="163"/>
+      <c r="I25" s="175"/>
       <c r="J25" s="66"/>
-      <c r="K25" s="165"/>
+      <c r="K25" s="177"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
@@ -5048,7 +5048,7 @@
       <c r="P25" s="2"/>
     </row>
     <row r="26" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="159"/>
+      <c r="A26" s="162"/>
       <c r="B26" s="2"/>
       <c r="C26" s="80"/>
       <c r="D26" s="80"/>
@@ -5066,7 +5066,7 @@
       <c r="P26" s="2"/>
     </row>
     <row r="27" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="160"/>
+      <c r="A27" s="163"/>
       <c r="B27" s="2"/>
       <c r="C27" s="68">
         <f>SUM(C23:C25)</f>
@@ -5146,7 +5146,7 @@
       <c r="P30" s="2"/>
     </row>
     <row r="31" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="158" t="s">
+      <c r="A31" s="161" t="s">
         <v>27</v>
       </c>
       <c r="B31" s="98" t="str">
@@ -5155,27 +5155,27 @@
       </c>
       <c r="C31" s="68">
         <f>Matrices!D35*Matrices!$N$35+Matrices!E35*Matrices!$N$36+Matrices!F35*Matrices!$N$37</f>
-        <v>0.24704184704184703</v>
+        <v>0.30707070707070705</v>
       </c>
       <c r="D31" s="66"/>
       <c r="E31" s="68">
         <f>IF(ISERROR(C31/Matrices!$N35),0,C31/Matrices!$N35)</f>
-        <v>3.0194003527336863</v>
+        <v>3.0412362749084987</v>
       </c>
       <c r="F31" s="66"/>
-      <c r="G31" s="161">
+      <c r="G31" s="173">
         <f>SUM(E31:E33)/Matrices!$B$15</f>
-        <v>3.1023190271515424</v>
+        <v>3.1918823994318823</v>
       </c>
       <c r="H31" s="66"/>
-      <c r="I31" s="161">
+      <c r="I31" s="173">
         <f>IF($C$35=Matrices!$B$15,0,(G31-Matrices!$B$15)/(Matrices!$B$15-1))</f>
-        <v>5.1159513575771198E-2</v>
+        <v>9.5941199715941172E-2</v>
       </c>
       <c r="J31" s="66"/>
-      <c r="K31" s="164">
+      <c r="K31" s="176">
         <f>IF(I31=0,0,I31/HLOOKUP(Matrices!$B$15,$R$6:$AA$7,2,0))</f>
-        <v>8.8206057889260697E-2</v>
+        <v>0.16541586157920893</v>
       </c>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
@@ -5184,26 +5184,26 @@
       <c r="P31" s="2"/>
     </row>
     <row r="32" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="159"/>
+      <c r="A32" s="162"/>
       <c r="B32" s="98" t="str">
         <f>B16</f>
         <v>Camellia-256-cbc</v>
       </c>
       <c r="C32" s="68">
         <f>Matrices!D36*Matrices!$N$35+Matrices!E36*Matrices!$N$36+Matrices!F36*Matrices!$N$37</f>
-        <v>0.54747474747474745</v>
+        <v>0.61709233253948703</v>
       </c>
       <c r="D32" s="66"/>
       <c r="E32" s="68">
         <f>IF(ISERROR(C32/Matrices!$N36),0,C32/Matrices!$N36)</f>
-        <v>3.0621468926553668</v>
+        <v>3.1290165868554376</v>
       </c>
       <c r="F32" s="66"/>
-      <c r="G32" s="162"/>
+      <c r="G32" s="174"/>
       <c r="H32" s="66"/>
-      <c r="I32" s="162"/>
+      <c r="I32" s="174"/>
       <c r="J32" s="66"/>
-      <c r="K32" s="165"/>
+      <c r="K32" s="177"/>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -5211,26 +5211,26 @@
       <c r="P32" s="2"/>
     </row>
     <row r="33" spans="1:27" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="159"/>
+      <c r="A33" s="162"/>
       <c r="B33" s="98" t="str">
         <f>B17</f>
         <v>Aes-256-cbc</v>
       </c>
       <c r="C33" s="68">
         <f>Matrices!D37*Matrices!$N$35+Matrices!E37*Matrices!$N$36+Matrices!F37*Matrices!$N$37</f>
-        <v>2.3848484848484848</v>
+        <v>2.3899564753223288</v>
       </c>
       <c r="D33" s="66"/>
       <c r="E33" s="68">
         <f>IF(ISERROR(C33/Matrices!$N37),0,C33/Matrices!$N37)</f>
-        <v>3.2254098360655736</v>
+        <v>3.4053943365317108</v>
       </c>
       <c r="F33" s="66"/>
-      <c r="G33" s="163"/>
+      <c r="G33" s="175"/>
       <c r="H33" s="66"/>
-      <c r="I33" s="163"/>
+      <c r="I33" s="175"/>
       <c r="J33" s="66"/>
-      <c r="K33" s="165"/>
+      <c r="K33" s="177"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -5249,7 +5249,7 @@
       <c r="AA33" s="2"/>
     </row>
     <row r="34" spans="1:27" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="159"/>
+      <c r="A34" s="162"/>
       <c r="B34" s="15"/>
       <c r="C34" s="80"/>
       <c r="D34" s="80"/>
@@ -5278,11 +5278,11 @@
       <c r="AA34" s="2"/>
     </row>
     <row r="35" spans="1:27" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="160"/>
+      <c r="A35" s="163"/>
       <c r="B35" s="2"/>
       <c r="C35" s="68">
         <f>SUM(C31:C33)</f>
-        <v>3.1793650793650792</v>
+        <v>3.3141195149325231</v>
       </c>
       <c r="D35" s="81"/>
       <c r="E35" s="81"/>
@@ -5378,7 +5378,7 @@
       <c r="O38" s="2"/>
     </row>
     <row r="39" spans="1:27" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="158" t="s">
+      <c r="A39" s="161" t="s">
         <v>27</v>
       </c>
       <c r="B39" s="99" t="str">
@@ -5395,17 +5395,17 @@
         <v>3.0044814914403517</v>
       </c>
       <c r="F39" s="66"/>
-      <c r="G39" s="161">
+      <c r="G39" s="173">
         <f>SUM(E39:E41)/Matrices!$B$15</f>
         <v>3.0218760598034478</v>
       </c>
       <c r="H39" s="66"/>
-      <c r="I39" s="161">
+      <c r="I39" s="173">
         <f>IF($C$43=Matrices!$B$15,0,(G39-Matrices!$B$15)/(Matrices!$B$15-1))</f>
         <v>1.0938029901723878E-2</v>
       </c>
       <c r="J39" s="66"/>
-      <c r="K39" s="164">
+      <c r="K39" s="176">
         <f>IF(I39=0,0,I39/HLOOKUP(Matrices!$B$15,$R$6:$AA$7,2,0))</f>
         <v>1.8858672244351515E-2</v>
       </c>
@@ -5415,7 +5415,7 @@
       <c r="O39" s="2"/>
     </row>
     <row r="40" spans="1:27" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="159"/>
+      <c r="A40" s="162"/>
       <c r="B40" s="99" t="str">
         <f>B16</f>
         <v>Camellia-256-cbc</v>
@@ -5430,18 +5430,18 @@
         <v>3.0094600008903529</v>
       </c>
       <c r="F40" s="66"/>
-      <c r="G40" s="162"/>
+      <c r="G40" s="174"/>
       <c r="H40" s="66"/>
-      <c r="I40" s="162"/>
+      <c r="I40" s="174"/>
       <c r="J40" s="66"/>
-      <c r="K40" s="165"/>
+      <c r="K40" s="177"/>
       <c r="L40" s="2"/>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
     </row>
     <row r="41" spans="1:27" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="159"/>
+      <c r="A41" s="162"/>
       <c r="B41" s="99" t="str">
         <f>B17</f>
         <v>Aes-256-cbc</v>
@@ -5456,18 +5456,18 @@
         <v>3.0516866870796373</v>
       </c>
       <c r="F41" s="66"/>
-      <c r="G41" s="163"/>
+      <c r="G41" s="175"/>
       <c r="H41" s="66"/>
-      <c r="I41" s="163"/>
+      <c r="I41" s="175"/>
       <c r="J41" s="66"/>
-      <c r="K41" s="165"/>
+      <c r="K41" s="177"/>
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
       <c r="O41" s="2"/>
     </row>
     <row r="42" spans="1:27" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="159"/>
+      <c r="A42" s="162"/>
       <c r="B42" s="2"/>
       <c r="C42" s="80"/>
       <c r="D42" s="80"/>
@@ -5484,7 +5484,7 @@
       <c r="O42" s="2"/>
     </row>
     <row r="43" spans="1:27" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="160"/>
+      <c r="A43" s="163"/>
       <c r="B43" s="2"/>
       <c r="C43" s="67">
         <f>SUM(C39:C41)</f>
@@ -6404,15 +6404,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="K15:K17"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A6:A11"/>
-    <mergeCell ref="G6:G9"/>
-    <mergeCell ref="I6:I9"/>
-    <mergeCell ref="K6:K9"/>
     <mergeCell ref="A39:A43"/>
     <mergeCell ref="G39:G41"/>
     <mergeCell ref="I39:I41"/>
@@ -6425,6 +6416,15 @@
     <mergeCell ref="G31:G33"/>
     <mergeCell ref="I31:I33"/>
     <mergeCell ref="K31:K33"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="K15:K17"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A6:A11"/>
+    <mergeCell ref="G6:G9"/>
+    <mergeCell ref="I6:I9"/>
+    <mergeCell ref="K6:K9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -6435,8 +6435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6451,24 +6451,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="36.6" x14ac:dyDescent="0.85">
-      <c r="A1" s="143" t="s">
+      <c r="A1" s="146" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="143"/>
-      <c r="C1" s="143"/>
-      <c r="D1" s="143"/>
-      <c r="E1" s="143"/>
-      <c r="F1" s="143"/>
-      <c r="G1" s="143"/>
-      <c r="H1" s="143"/>
-      <c r="I1" s="143"/>
-      <c r="J1" s="143"/>
-      <c r="K1" s="143"/>
-      <c r="L1" s="143"/>
-      <c r="M1" s="143"/>
-      <c r="N1" s="143"/>
-      <c r="O1" s="143"/>
-      <c r="P1" s="143"/>
+      <c r="B1" s="146"/>
+      <c r="C1" s="146"/>
+      <c r="D1" s="146"/>
+      <c r="E1" s="146"/>
+      <c r="F1" s="146"/>
+      <c r="G1" s="146"/>
+      <c r="H1" s="146"/>
+      <c r="I1" s="146"/>
+      <c r="J1" s="146"/>
+      <c r="K1" s="146"/>
+      <c r="L1" s="146"/>
+      <c r="M1" s="146"/>
+      <c r="N1" s="146"/>
+      <c r="O1" s="146"/>
+      <c r="P1" s="146"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
@@ -6546,16 +6546,16 @@
     </row>
     <row r="6" spans="1:16" ht="18.600000000000001" x14ac:dyDescent="0.45">
       <c r="A6" s="2"/>
-      <c r="B6" s="175" t="s">
+      <c r="B6" s="178" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="176"/>
-      <c r="D6" s="176"/>
-      <c r="E6" s="176"/>
-      <c r="F6" s="177"/>
+      <c r="C6" s="179"/>
+      <c r="D6" s="179"/>
+      <c r="E6" s="179"/>
+      <c r="F6" s="180"/>
       <c r="G6" s="124"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="178" t="s">
+      <c r="I6" s="181" t="s">
         <v>30</v>
       </c>
       <c r="J6" s="41"/>
@@ -6575,7 +6575,7 @@
       <c r="F7" s="42"/>
       <c r="G7" s="42"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="179"/>
+      <c r="I7" s="182"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
@@ -6587,15 +6587,15 @@
     <row r="8" spans="1:16" ht="16.2" x14ac:dyDescent="0.4">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
-      <c r="C8" s="181" t="s">
+      <c r="C8" s="184" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="181"/>
-      <c r="E8" s="181"/>
-      <c r="F8" s="181"/>
+      <c r="D8" s="184"/>
+      <c r="E8" s="184"/>
+      <c r="F8" s="184"/>
       <c r="G8" s="109"/>
       <c r="H8" s="2"/>
-      <c r="I8" s="180"/>
+      <c r="I8" s="183"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
@@ -6647,7 +6647,7 @@
       </c>
       <c r="E10" s="83">
         <f>Matrices!N35</f>
-        <v>8.1818181818181804E-2</v>
+        <v>0.10096903999343025</v>
       </c>
       <c r="F10" s="83">
         <f>Matrices!N44</f>
@@ -6660,7 +6660,7 @@
       </c>
       <c r="I10" s="118">
         <f>SUMPRODUCT(C10:F10,$C$14:$F$14)</f>
-        <v>0.48678146580420634</v>
+        <v>0.4888258929296686</v>
       </c>
       <c r="J10" s="104" t="str">
         <f>IF(I10=MAX($I$10:$I$12),"&lt;=MEJOR ALTERNATIVA","")</f>
@@ -6685,7 +6685,7 @@
       </c>
       <c r="E11" s="83">
         <f>Matrices!N36</f>
-        <v>0.1787878787878788</v>
+        <v>0.19721606306972161</v>
       </c>
       <c r="F11" s="83">
         <f>Matrices!N45</f>
@@ -6698,7 +6698,7 @@
       </c>
       <c r="I11" s="118">
         <f>SUMPRODUCT(C11:F11,$C$14:$F$14)</f>
-        <v>0.16433669763498304</v>
+        <v>0.16630397656703164</v>
       </c>
       <c r="J11" s="105" t="str">
         <f>IF(I11=MAX($I$10:$I$12),"&lt;=MEJOR ALTERNATIVA","")</f>
@@ -6723,7 +6723,7 @@
       </c>
       <c r="E12" s="83">
         <f>Matrices!N37</f>
-        <v>0.73939393939393938</v>
+        <v>0.70181489693684806</v>
       </c>
       <c r="F12" s="83">
         <f>Matrices!N46</f>
@@ -6736,7 +6736,7 @@
       </c>
       <c r="I12" s="119">
         <f>SUMPRODUCT(C12:F12,$C$14:$F$14)</f>
-        <v>0.34888183656081062</v>
+        <v>0.34487013050329979</v>
       </c>
       <c r="J12" s="105" t="str">
         <f>IF(I12=MAX($I$10:$I$12),"&lt;=MEJOR ALTERNATIVA","")</f>
@@ -6811,9 +6811,9 @@
       <c r="F16" s="41"/>
       <c r="G16" s="41"/>
       <c r="H16" s="2"/>
-      <c r="I16" s="182"/>
-      <c r="J16" s="182"/>
-      <c r="K16" s="182"/>
+      <c r="I16" s="185"/>
+      <c r="J16" s="185"/>
+      <c r="K16" s="185"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>

</xml_diff>